<commit_message>
New Page Code Done
</commit_message>
<xml_diff>
--- a/Content Check Dipen bhai/Page Urls.xlsx
+++ b/Content Check Dipen bhai/Page Urls.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B777EDDB-DABE-436B-A8B7-D6B8C44316CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="86">
   <si>
     <t>Page No.</t>
   </si>
@@ -380,11 +381,14 @@
       <t>.</t>
     </r>
   </si>
+  <si>
+    <t>https://answerthepublic.com/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -748,11 +752,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -765,7 +769,7 @@
     <col min="7" max="7" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="60.75" thickBot="1">
+    <row r="1" spans="1:7" ht="30.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1131,6 +1135,11 @@
       </c>
       <c r="G16" s="4" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>